<commit_message>
Added the visualisations into my website and made final edits
</commit_message>
<xml_diff>
--- a/EXCEL DATA.xlsx
+++ b/EXCEL DATA.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d2092b68edc9030/Documents/MAJOR PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{22D15A3A-4D17-44ED-BFFC-6EAEE6B5A32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D57FE3B-705E-4717-B8EE-D14909819B35}"/>
+  <xr:revisionPtr revIDLastSave="648" documentId="8_{22D15A3A-4D17-44ED-BFFC-6EAEE6B5A32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94FA9095-E757-409D-94AA-AE971C5E5101}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{26B9F8EF-3941-4B03-9B24-99A57DD27147}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{26B9F8EF-3941-4B03-9B24-99A57DD27147}"/>
   </bookViews>
   <sheets>
-    <sheet name="Math Grade Improvement" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Grade Improvement" sheetId="3" r:id="rId2"/>
+    <sheet name="S1 VS S2" sheetId="4" r:id="rId3"/>
+    <sheet name="Grade Average " sheetId="5" r:id="rId4"/>
+    <sheet name="CTL vs Grade Average" sheetId="6" r:id="rId5"/>
+    <sheet name="Time Spent Per Student" sheetId="8" r:id="rId6"/>
+    <sheet name="Scatter Plot" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="26">
   <si>
     <t>Student Name</t>
   </si>
@@ -88,6 +93,33 @@
   </si>
   <si>
     <t>Grade Improvement</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Average Grade</t>
+  </si>
+  <si>
+    <t>Grade Average</t>
+  </si>
+  <si>
+    <t>Time Spent (Hours)</t>
+  </si>
+  <si>
+    <t>Total Time Spent (Hours)</t>
+  </si>
+  <si>
+    <t>Student 3</t>
+  </si>
+  <si>
+    <t>Grade Improvement (%)</t>
   </si>
 </sst>
 </file>
@@ -123,8 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E55D2DD-90CB-483D-89C0-3A1078B21AC1}">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="J11" sqref="H2:J11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +510,7 @@
     <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
@@ -485,7 +519,7 @@
     <col min="13" max="13" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -501,17 +535,11 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -522,23 +550,16 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <f>E4-E3</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -554,18 +575,11 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <f>E6-E5</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -576,23 +590,16 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5">
-        <f>E8-E7</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -608,18 +615,11 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <f>E10-E9</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -630,23 +630,16 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7">
-        <f>E12-E11</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -662,18 +655,11 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8">
-        <f>E14-E13</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -684,23 +670,16 @@
         <v>6</v>
       </c>
       <c r="E9">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9">
-        <f>E16-E15</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -714,20 +693,13 @@
         <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10">
-        <f>E18-E17</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -738,23 +710,16 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11">
-        <f>E20-E19</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -770,8 +735,11 @@
       <c r="F12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -782,13 +750,16 @@
         <v>12</v>
       </c>
       <c r="E13">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -802,10 +773,13 @@
         <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -816,13 +790,16 @@
         <v>6</v>
       </c>
       <c r="E15">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -838,8 +815,11 @@
       <c r="F16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -850,13 +830,16 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -872,8 +855,11 @@
       <c r="F18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -884,13 +870,16 @@
         <v>12</v>
       </c>
       <c r="E19">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -905,6 +894,9 @@
       </c>
       <c r="F20" t="s">
         <v>9</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -921,11 +913,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4119567C-279F-410D-91B1-EDE1428B61CC}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -946,8 +942,8 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <f>'Math Grade Improvement'!E4-'Math Grade Improvement'!E3</f>
-        <v>6</v>
+        <f>'Raw Data'!E4-'Raw Data'!E3</f>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -958,8 +954,8 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <f>'Math Grade Improvement'!E6-'Math Grade Improvement'!E5</f>
-        <v>6</v>
+        <f>'Raw Data'!E6-'Raw Data'!E5</f>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -970,8 +966,8 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <f>'Math Grade Improvement'!E8-'Math Grade Improvement'!E7</f>
-        <v>4</v>
+        <f>'Raw Data'!E8-'Raw Data'!E7</f>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -982,8 +978,8 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <f>'Math Grade Improvement'!E10-'Math Grade Improvement'!E9</f>
-        <v>14</v>
+        <f>'Raw Data'!E10-'Raw Data'!E9</f>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -994,8 +990,8 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <f>'Math Grade Improvement'!E12-'Math Grade Improvement'!E11</f>
-        <v>9</v>
+        <f>'Raw Data'!E12-'Raw Data'!E11</f>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1006,8 +1002,8 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <f>'Math Grade Improvement'!E14-'Math Grade Improvement'!E13</f>
-        <v>12</v>
+        <f>'Raw Data'!E14-'Raw Data'!E13</f>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1018,8 +1014,8 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <f>'Math Grade Improvement'!E16-'Math Grade Improvement'!E15</f>
-        <v>10</v>
+        <f>'Raw Data'!E16-'Raw Data'!E15</f>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1030,8 +1026,8 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <f>'Math Grade Improvement'!E18-'Math Grade Improvement'!E17</f>
-        <v>7</v>
+        <f>'Raw Data'!E18-'Raw Data'!E17</f>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1042,8 +1038,707 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <f>'Math Grade Improvement'!E20-'Math Grade Improvement'!E19</f>
-        <v>6</v>
+        <f>'Raw Data'!E20-'Raw Data'!E19</f>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3D6009-3FCF-4CFF-8B6B-545DD22E0545}">
+  <dimension ref="B2:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42DBA26-7B4B-4126-9D39-AC8AE7CB23B4}">
+  <dimension ref="B2:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <f>AVERAGE('Raw Data'!E3,'Raw Data'!E9,'Raw Data'!E15)</f>
+        <v>58.333333333333336</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <f>AVERAGE('Raw Data'!E4,'Raw Data'!E10,'Raw Data'!E16)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <f>AVERAGE('Raw Data'!E5,'Raw Data'!E11,'Raw Data'!E17)</f>
+        <v>55.666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <f>AVERAGE('Raw Data'!E6,'Raw Data'!E12,'Raw Data'!E18)</f>
+        <v>83.333333333333329</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1">
+        <f>AVERAGE('Raw Data'!E7,'Raw Data'!E13,'Raw Data'!E19)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
+        <f>AVERAGE('Raw Data'!E8,'Raw Data'!E14,'Raw Data'!E20)</f>
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1697DBA7-69D1-4596-ADF7-2042905A01E4}">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <f>AVERAGE('Raw Data'!E9,'Raw Data'!E11,'Raw Data'!E13,'Raw Data'!E17)</f>
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <f>AVERAGE('Raw Data'!E3,'Raw Data'!E5,'Raw Data'!E7,'Raw Data'!E15,'Raw Data'!E16,'Raw Data'!E18,'Raw Data'!E19,'Raw Data'!E20)</f>
+        <v>68.625</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <f>AVERAGE('Raw Data'!E4,'Raw Data'!E6,'Raw Data'!E8,'Raw Data'!E10,'Raw Data'!E12,'Raw Data'!E14)</f>
+        <v>86.833333333333329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38B869-3CB6-420C-8E8E-5D9CA3DE368D}">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <f>SUM('Raw Data'!G3,'Raw Data'!G4,'Raw Data'!G5,'Raw Data'!G6,'Raw Data'!G7,'Raw Data'!G8)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f>SUM('Raw Data'!G9,'Raw Data'!G10,'Raw Data'!G11,'Raw Data'!G12,'Raw Data'!G13,'Raw Data'!G14)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <f>SUM('Raw Data'!G15,'Raw Data'!G16,'Raw Data'!G17,'Raw Data'!G18,'Raw Data'!G19,'Raw Data'!G20)</f>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B796B17D-5A8E-4D0A-8B45-BD9328215D56}">
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f>'Raw Data'!E4-'Raw Data'!E3</f>
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <f>'Raw Data'!E6-'Raw Data'!E5</f>
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <f>'Raw Data'!E8-'Raw Data'!E7</f>
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f>'Raw Data'!E10-'Raw Data'!E9</f>
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <f>'Raw Data'!E12-'Raw Data'!E11</f>
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <f>'Raw Data'!E14-'Raw Data'!E13</f>
+        <v>41</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f>'Raw Data'!E16-'Raw Data'!E15</f>
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <f>'Raw Data'!E18-'Raw Data'!E17</f>
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <f>'Raw Data'!E20-'Raw Data'!E19</f>
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>